<commit_message>
Address issues in PR review for Excel tests automation
</commit_message>
<xml_diff>
--- a/test/core/excel/WriteToReadOnlyFile.xlsx
+++ b/test/core/excel/WriteToReadOnlyFile.xlsx
@@ -336,43 +336,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>